<commit_message>
derive mspatient from us-core-patient
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-ms-bundle-hla-multilocus.xlsx
+++ b/docs/StructureDefinition-ms-bundle-hla-multilocus.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-10-31T18:02:56-05:00</t>
+    <t>2022-11-02T14:44:07-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1122,7 +1122,7 @@
     <t>Information about an individual or animal receiving health care services</t>
   </si>
   <si>
-    <t>Demographics and other administrative information about an individual or animal receiving care or other health-related services.</t>
+    <t>The US Core Patient Profile is based upon the core FHIR Patient Resource and designed to meet the applicable patient demographic data elements from the 2015 Edition Common Clinical Data Set.</t>
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}

</xml_diff>

<commit_message>
removed NMDP race and ethnicity codes
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-ms-bundle-hla-multilocus.xlsx
+++ b/docs/StructureDefinition-ms-bundle-hla-multilocus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15602" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15602" uniqueCount="437">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-11-02T14:44:07-05:00</t>
+    <t>2022-12-01T09:35:21-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1126,7 +1126,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}rac-1:Shall use either NMDP Race extension or us-core-race {extension.exists(url = 'http://fhir.nmdp.org/ig/matchsource/StructureDefinition/nmdp-race' or url = 'http://hl7.org/fhir/us/core/StructureDefinition/us-core-race')}eth-1:Shall use either NMDP ethnicity extension or us-core-ethnicity {extension.exists(url = 'http://fhir.nmdp.org/ig/matchsource/StructureDefinition/nmdp-ethnicity' or url = 'http://hl7.org/fhir/us/core/StructureDefinition/us-core-ethnicity')}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>Patient[classCode=PAT]</t>
@@ -1181,10 +1181,6 @@
   </si>
   <si>
     <t>A person who is directly or indirectly involved in the provisioning of healthcare.</t>
-  </si>
-  <si>
-    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
     <t>PRD (as one example)</t>
@@ -16649,13 +16645,13 @@
         <v>74</v>
       </c>
       <c r="AI135" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="AJ135" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="AJ135" t="s" s="2">
+      <c r="AK135" t="s" s="2">
         <v>373</v>
-      </c>
-      <c r="AK135" t="s" s="2">
-        <v>374</v>
       </c>
       <c r="AL135" t="s" s="2">
         <v>74</v>
@@ -19424,7 +19420,7 @@
         <v>256</v>
       </c>
       <c r="B161" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C161" t="s" s="2">
         <v>74</v>
@@ -19449,10 +19445,10 @@
         <v>238</v>
       </c>
       <c r="K161" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L161" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="M161" s="2"/>
       <c r="N161" s="2"/>
@@ -20108,13 +20104,13 @@
         <v>74</v>
       </c>
       <c r="J167" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="K167" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="K167" t="s" s="2">
+      <c r="L167" t="s" s="2">
         <v>378</v>
-      </c>
-      <c r="L167" t="s" s="2">
-        <v>379</v>
       </c>
       <c r="M167" s="2"/>
       <c r="N167" s="2"/>
@@ -20177,13 +20173,13 @@
         <v>74</v>
       </c>
       <c r="AI167" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="AJ167" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="AJ167" t="s" s="2">
+      <c r="AK167" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="AK167" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="AL167" t="s" s="2">
         <v>74</v>
@@ -22952,7 +22948,7 @@
         <v>256</v>
       </c>
       <c r="B193" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C193" t="s" s="2">
         <v>74</v>
@@ -22977,10 +22973,10 @@
         <v>238</v>
       </c>
       <c r="K193" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="L193" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="L193" t="s" s="2">
-        <v>385</v>
       </c>
       <c r="M193" s="2"/>
       <c r="N193" s="2"/>
@@ -23617,7 +23613,7 @@
       </c>
       <c r="B199" s="2"/>
       <c r="C199" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D199" s="2"/>
       <c r="E199" t="s" s="2">
@@ -23636,16 +23632,16 @@
         <v>74</v>
       </c>
       <c r="J199" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="K199" t="s" s="2">
         <v>387</v>
       </c>
-      <c r="K199" t="s" s="2">
+      <c r="L199" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="L199" t="s" s="2">
+      <c r="M199" t="s" s="2">
         <v>389</v>
-      </c>
-      <c r="M199" t="s" s="2">
-        <v>390</v>
       </c>
       <c r="N199" s="2"/>
       <c r="O199" t="s" s="2">
@@ -23707,13 +23703,13 @@
         <v>74</v>
       </c>
       <c r="AI199" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AJ199" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="AJ199" t="s" s="2">
+      <c r="AK199" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="AK199" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="AL199" t="s" s="2">
         <v>74</v>
@@ -26482,7 +26478,7 @@
         <v>256</v>
       </c>
       <c r="B225" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C225" t="s" s="2">
         <v>74</v>
@@ -26507,10 +26503,10 @@
         <v>238</v>
       </c>
       <c r="K225" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="L225" t="s" s="2">
         <v>395</v>
-      </c>
-      <c r="L225" t="s" s="2">
-        <v>396</v>
       </c>
       <c r="M225" s="2"/>
       <c r="N225" s="2"/>
@@ -27147,7 +27143,7 @@
       </c>
       <c r="B231" s="2"/>
       <c r="C231" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D231" s="2"/>
       <c r="E231" t="s" s="2">
@@ -27166,16 +27162,16 @@
         <v>74</v>
       </c>
       <c r="J231" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K231" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L231" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="L231" t="s" s="2">
+      <c r="M231" t="s" s="2">
         <v>389</v>
-      </c>
-      <c r="M231" t="s" s="2">
-        <v>390</v>
       </c>
       <c r="N231" s="2"/>
       <c r="O231" t="s" s="2">
@@ -27237,13 +27233,13 @@
         <v>74</v>
       </c>
       <c r="AI231" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AJ231" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="AJ231" t="s" s="2">
+      <c r="AK231" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="AK231" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="AL231" t="s" s="2">
         <v>74</v>
@@ -30012,7 +30008,7 @@
         <v>256</v>
       </c>
       <c r="B257" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C257" t="s" s="2">
         <v>74</v>
@@ -30037,10 +30033,10 @@
         <v>238</v>
       </c>
       <c r="K257" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="L257" t="s" s="2">
         <v>399</v>
-      </c>
-      <c r="L257" t="s" s="2">
-        <v>400</v>
       </c>
       <c r="M257" s="2"/>
       <c r="N257" s="2"/>
@@ -30677,7 +30673,7 @@
       </c>
       <c r="B263" s="2"/>
       <c r="C263" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D263" s="2"/>
       <c r="E263" t="s" s="2">
@@ -30696,16 +30692,16 @@
         <v>74</v>
       </c>
       <c r="J263" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K263" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L263" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="L263" t="s" s="2">
+      <c r="M263" t="s" s="2">
         <v>389</v>
-      </c>
-      <c r="M263" t="s" s="2">
-        <v>390</v>
       </c>
       <c r="N263" s="2"/>
       <c r="O263" t="s" s="2">
@@ -30767,13 +30763,13 @@
         <v>74</v>
       </c>
       <c r="AI263" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AJ263" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="AJ263" t="s" s="2">
+      <c r="AK263" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="AK263" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="AL263" t="s" s="2">
         <v>74</v>
@@ -33542,7 +33538,7 @@
         <v>256</v>
       </c>
       <c r="B289" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C289" t="s" s="2">
         <v>74</v>
@@ -33567,10 +33563,10 @@
         <v>238</v>
       </c>
       <c r="K289" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L289" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M289" s="2"/>
       <c r="N289" s="2"/>
@@ -34207,7 +34203,7 @@
       </c>
       <c r="B295" s="2"/>
       <c r="C295" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D295" s="2"/>
       <c r="E295" t="s" s="2">
@@ -34226,16 +34222,16 @@
         <v>74</v>
       </c>
       <c r="J295" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K295" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L295" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="L295" t="s" s="2">
+      <c r="M295" t="s" s="2">
         <v>389</v>
-      </c>
-      <c r="M295" t="s" s="2">
-        <v>390</v>
       </c>
       <c r="N295" s="2"/>
       <c r="O295" t="s" s="2">
@@ -34297,13 +34293,13 @@
         <v>74</v>
       </c>
       <c r="AI295" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AJ295" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="AJ295" t="s" s="2">
+      <c r="AK295" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="AK295" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="AL295" t="s" s="2">
         <v>74</v>
@@ -37072,7 +37068,7 @@
         <v>256</v>
       </c>
       <c r="B321" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C321" t="s" s="2">
         <v>74</v>
@@ -37097,10 +37093,10 @@
         <v>238</v>
       </c>
       <c r="K321" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="L321" t="s" s="2">
         <v>406</v>
-      </c>
-      <c r="L321" t="s" s="2">
-        <v>407</v>
       </c>
       <c r="M321" s="2"/>
       <c r="N321" s="2"/>
@@ -37737,7 +37733,7 @@
       </c>
       <c r="B327" s="2"/>
       <c r="C327" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D327" s="2"/>
       <c r="E327" t="s" s="2">
@@ -37756,16 +37752,16 @@
         <v>74</v>
       </c>
       <c r="J327" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="K327" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="K327" t="s" s="2">
+      <c r="L327" t="s" s="2">
         <v>409</v>
       </c>
-      <c r="L327" t="s" s="2">
-        <v>410</v>
-      </c>
       <c r="M327" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="N327" s="2"/>
       <c r="O327" t="s" s="2">
@@ -37827,13 +37823,13 @@
         <v>74</v>
       </c>
       <c r="AI327" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AJ327" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="AK327" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="AK327" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="AL327" t="s" s="2">
         <v>74</v>
@@ -40602,7 +40598,7 @@
         <v>256</v>
       </c>
       <c r="B353" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C353" t="s" s="2">
         <v>74</v>
@@ -40627,10 +40623,10 @@
         <v>238</v>
       </c>
       <c r="K353" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="L353" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="L353" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="M353" s="2"/>
       <c r="N353" s="2"/>
@@ -41267,7 +41263,7 @@
       </c>
       <c r="B359" s="2"/>
       <c r="C359" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D359" s="2"/>
       <c r="E359" t="s" s="2">
@@ -41286,16 +41282,16 @@
         <v>74</v>
       </c>
       <c r="J359" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="K359" t="s" s="2">
         <v>415</v>
       </c>
-      <c r="K359" t="s" s="2">
+      <c r="L359" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="L359" t="s" s="2">
-        <v>417</v>
-      </c>
       <c r="M359" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="N359" s="2"/>
       <c r="O359" t="s" s="2">
@@ -41357,13 +41353,13 @@
         <v>74</v>
       </c>
       <c r="AI359" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AJ359" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="AK359" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="AK359" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="AL359" t="s" s="2">
         <v>74</v>
@@ -44132,7 +44128,7 @@
         <v>256</v>
       </c>
       <c r="B385" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C385" t="s" s="2">
         <v>74</v>
@@ -44157,10 +44153,10 @@
         <v>238</v>
       </c>
       <c r="K385" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="L385" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="L385" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="M385" s="2"/>
       <c r="N385" s="2"/>
@@ -44816,13 +44812,13 @@
         <v>74</v>
       </c>
       <c r="J391" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="K391" t="s" s="2">
         <v>421</v>
       </c>
-      <c r="K391" t="s" s="2">
+      <c r="L391" t="s" s="2">
         <v>422</v>
-      </c>
-      <c r="L391" t="s" s="2">
-        <v>423</v>
       </c>
       <c r="M391" s="2"/>
       <c r="N391" s="2"/>
@@ -44885,13 +44881,13 @@
         <v>74</v>
       </c>
       <c r="AI391" t="s" s="2">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="AJ391" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AK391" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AL391" t="s" s="2">
         <v>74</v>
@@ -47660,7 +47656,7 @@
         <v>256</v>
       </c>
       <c r="B417" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C417" t="s" s="2">
         <v>74</v>
@@ -47685,10 +47681,10 @@
         <v>238</v>
       </c>
       <c r="K417" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="L417" t="s" s="2">
         <v>426</v>
-      </c>
-      <c r="L417" t="s" s="2">
-        <v>427</v>
       </c>
       <c r="M417" s="2"/>
       <c r="N417" s="2"/>
@@ -48325,7 +48321,7 @@
       </c>
       <c r="B423" s="2"/>
       <c r="C423" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D423" s="2"/>
       <c r="E423" t="s" s="2">
@@ -48344,16 +48340,16 @@
         <v>74</v>
       </c>
       <c r="J423" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="K423" t="s" s="2">
         <v>428</v>
       </c>
-      <c r="K423" t="s" s="2">
+      <c r="L423" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="L423" t="s" s="2">
+      <c r="M423" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="M423" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="N423" s="2"/>
       <c r="O423" t="s" s="2">
@@ -48415,13 +48411,13 @@
         <v>74</v>
       </c>
       <c r="AI423" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AJ423" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="AJ423" t="s" s="2">
+      <c r="AK423" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="AK423" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="AL423" t="s" s="2">
         <v>74</v>
@@ -51187,7 +51183,7 @@
     </row>
     <row r="449" hidden="true">
       <c r="A449" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B449" s="2"/>
       <c r="C449" t="s" s="2">
@@ -51210,19 +51206,19 @@
         <v>83</v>
       </c>
       <c r="J449" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="K449" t="s" s="2">
         <v>433</v>
       </c>
-      <c r="K449" t="s" s="2">
+      <c r="L449" t="s" s="2">
         <v>434</v>
       </c>
-      <c r="L449" t="s" s="2">
+      <c r="M449" t="s" s="2">
         <v>435</v>
       </c>
-      <c r="M449" t="s" s="2">
+      <c r="N449" t="s" s="2">
         <v>436</v>
-      </c>
-      <c r="N449" t="s" s="2">
-        <v>437</v>
       </c>
       <c r="O449" t="s" s="2">
         <v>74</v>
@@ -51271,7 +51267,7 @@
         <v>74</v>
       </c>
       <c r="AE449" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AF449" t="s" s="2">
         <v>75</v>

</xml_diff>

<commit_message>
added publication dirs; changed package id
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-ms-bundle-hla-multilocus.xlsx
+++ b/docs/StructureDefinition-ms-bundle-hla-multilocus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17191" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17191" uniqueCount="867">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-06T10:47:25-05:00</t>
+    <t>2023-05-09T13:12:05-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2588,12 +2588,6 @@
   </si>
   <si>
     <t>Genotype</t>
-  </si>
-  <si>
-    <t>A finding that a patient has a specific genotype.</t>
-  </si>
-  <si>
-    <t>Defines those properties that are common for all findings of genetic characteristics - namely genotype, haplotype and any of the types of variants.</t>
   </si>
   <si>
     <t>Bundle.entry:hla-multi.search</t>
@@ -54522,7 +54516,7 @@
         <v>84</v>
       </c>
       <c r="H455" t="s" s="2">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="I455" t="s" s="2">
         <v>75</v>
@@ -54537,10 +54531,10 @@
         <v>835</v>
       </c>
       <c r="M455" t="s" s="2">
-        <v>836</v>
+        <v>571</v>
       </c>
       <c r="N455" t="s" s="2">
-        <v>837</v>
+        <v>572</v>
       </c>
       <c r="O455" s="2"/>
       <c r="P455" t="s" s="2">
@@ -54619,7 +54613,7 @@
     </row>
     <row r="456" hidden="true">
       <c r="A456" t="s" s="2">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B456" t="s" s="2">
         <v>287</v>
@@ -54731,7 +54725,7 @@
     </row>
     <row r="457" hidden="true">
       <c r="A457" t="s" s="2">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B457" t="s" s="2">
         <v>291</v>
@@ -54843,7 +54837,7 @@
     </row>
     <row r="458" hidden="true">
       <c r="A458" t="s" s="2">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B458" t="s" s="2">
         <v>292</v>
@@ -54957,7 +54951,7 @@
     </row>
     <row r="459" hidden="true">
       <c r="A459" t="s" s="2">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B459" t="s" s="2">
         <v>293</v>
@@ -55073,7 +55067,7 @@
     </row>
     <row r="460" hidden="true">
       <c r="A460" t="s" s="2">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B460" t="s" s="2">
         <v>294</v>
@@ -55187,7 +55181,7 @@
     </row>
     <row r="461" hidden="true">
       <c r="A461" t="s" s="2">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B461" t="s" s="2">
         <v>300</v>
@@ -55301,7 +55295,7 @@
     </row>
     <row r="462" hidden="true">
       <c r="A462" t="s" s="2">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B462" t="s" s="2">
         <v>305</v>
@@ -55413,7 +55407,7 @@
     </row>
     <row r="463" hidden="true">
       <c r="A463" t="s" s="2">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="B463" t="s" s="2">
         <v>309</v>
@@ -55525,7 +55519,7 @@
     </row>
     <row r="464" hidden="true">
       <c r="A464" t="s" s="2">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B464" t="s" s="2">
         <v>310</v>
@@ -55639,7 +55633,7 @@
     </row>
     <row r="465" hidden="true">
       <c r="A465" t="s" s="2">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="B465" t="s" s="2">
         <v>311</v>
@@ -55755,7 +55749,7 @@
     </row>
     <row r="466" hidden="true">
       <c r="A466" t="s" s="2">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B466" t="s" s="2">
         <v>312</v>
@@ -55867,7 +55861,7 @@
     </row>
     <row r="467" hidden="true">
       <c r="A467" t="s" s="2">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="B467" t="s" s="2">
         <v>317</v>
@@ -55981,7 +55975,7 @@
     </row>
     <row r="468" hidden="true">
       <c r="A468" t="s" s="2">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B468" t="s" s="2">
         <v>321</v>
@@ -56093,7 +56087,7 @@
     </row>
     <row r="469" hidden="true">
       <c r="A469" t="s" s="2">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="B469" t="s" s="2">
         <v>324</v>
@@ -56205,7 +56199,7 @@
     </row>
     <row r="470" hidden="true">
       <c r="A470" t="s" s="2">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B470" t="s" s="2">
         <v>326</v>
@@ -56317,7 +56311,7 @@
     </row>
     <row r="471" hidden="true">
       <c r="A471" t="s" s="2">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="B471" t="s" s="2">
         <v>329</v>
@@ -56429,7 +56423,7 @@
     </row>
     <row r="472" hidden="true">
       <c r="A472" t="s" s="2">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="B472" t="s" s="2">
         <v>332</v>
@@ -56541,7 +56535,7 @@
     </row>
     <row r="473" hidden="true">
       <c r="A473" t="s" s="2">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="B473" t="s" s="2">
         <v>336</v>
@@ -56653,7 +56647,7 @@
     </row>
     <row r="474" hidden="true">
       <c r="A474" t="s" s="2">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B474" t="s" s="2">
         <v>337</v>
@@ -56767,7 +56761,7 @@
     </row>
     <row r="475" hidden="true">
       <c r="A475" t="s" s="2">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="B475" t="s" s="2">
         <v>338</v>
@@ -56883,7 +56877,7 @@
     </row>
     <row r="476" hidden="true">
       <c r="A476" t="s" s="2">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B476" t="s" s="2">
         <v>339</v>
@@ -56995,7 +56989,7 @@
     </row>
     <row r="477" hidden="true">
       <c r="A477" t="s" s="2">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B477" t="s" s="2">
         <v>342</v>
@@ -57107,7 +57101,7 @@
     </row>
     <row r="478" hidden="true">
       <c r="A478" t="s" s="2">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B478" t="s" s="2">
         <v>345</v>
@@ -57221,7 +57215,7 @@
     </row>
     <row r="479" hidden="true">
       <c r="A479" t="s" s="2">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B479" t="s" s="2">
         <v>349</v>
@@ -57335,7 +57329,7 @@
     </row>
     <row r="480" hidden="true">
       <c r="A480" t="s" s="2">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B480" t="s" s="2">
         <v>353</v>
@@ -57449,10 +57443,10 @@
     </row>
     <row r="481" hidden="true">
       <c r="A481" t="s" s="2">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="B481" t="s" s="2">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="C481" s="2"/>
       <c r="D481" t="s" s="2">
@@ -57475,19 +57469,19 @@
         <v>85</v>
       </c>
       <c r="K481" t="s" s="2">
+        <v>862</v>
+      </c>
+      <c r="L481" t="s" s="2">
+        <v>863</v>
+      </c>
+      <c r="M481" t="s" s="2">
         <v>864</v>
       </c>
-      <c r="L481" t="s" s="2">
+      <c r="N481" t="s" s="2">
         <v>865</v>
       </c>
-      <c r="M481" t="s" s="2">
+      <c r="O481" t="s" s="2">
         <v>866</v>
-      </c>
-      <c r="N481" t="s" s="2">
-        <v>867</v>
-      </c>
-      <c r="O481" t="s" s="2">
-        <v>868</v>
       </c>
       <c r="P481" t="s" s="2">
         <v>75</v>
@@ -57536,7 +57530,7 @@
         <v>75</v>
       </c>
       <c r="AF481" t="s" s="2">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="AG481" t="s" s="2">
         <v>76</v>

</xml_diff>